<commit_message>
Final commit for project 4
</commit_message>
<xml_diff>
--- a/Connected Office Web Application User Acceptance Test/Connected Office Test Data.xlsx
+++ b/Connected Office Web Application User Acceptance Test/Connected Office Test Data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marcel\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marcel\Desktop\323 P4\CMPG-323-Project-4---35376759\Connected Office Web Application User Acceptance Test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EB7CAE2-D38B-40BB-B3D6-CAFA324872CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B7A91DB-3554-421D-A5A6-A29A7E2D1E39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1185" yWindow="2040" windowWidth="23850" windowHeight="11295" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Device" sheetId="1" r:id="rId1"/>
@@ -1126,7 +1126,7 @@
   <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1159,16 +1159,16 @@
         <v>57</v>
       </c>
       <c r="B2" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D2" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E2" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1176,16 +1176,16 @@
         <v>58</v>
       </c>
       <c r="B3" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C3" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D3" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E3" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -1193,16 +1193,16 @@
         <v>59</v>
       </c>
       <c r="B4" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C4" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D4" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E4" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1210,16 +1210,16 @@
         <v>60</v>
       </c>
       <c r="B5" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C5" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D5" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E5" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -1227,16 +1227,16 @@
         <v>61</v>
       </c>
       <c r="B6" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C6" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D6" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E6" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -1244,16 +1244,16 @@
         <v>62</v>
       </c>
       <c r="B7" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C7" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D7" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E7" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -1261,16 +1261,16 @@
         <v>63</v>
       </c>
       <c r="B8" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C8" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D8" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E8" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -1278,16 +1278,16 @@
         <v>64</v>
       </c>
       <c r="B9" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C9" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D9" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E9" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -1295,16 +1295,16 @@
         <v>65</v>
       </c>
       <c r="B10" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C10" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D10" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E10" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -1312,16 +1312,16 @@
         <v>66</v>
       </c>
       <c r="B11" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C11" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D11" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E11" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -1329,16 +1329,16 @@
         <v>67</v>
       </c>
       <c r="B12" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C12" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D12" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E12" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -1346,16 +1346,16 @@
         <v>68</v>
       </c>
       <c r="B13" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C13" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D13" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E13" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -1363,16 +1363,16 @@
         <v>69</v>
       </c>
       <c r="B14" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C14" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D14" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E14" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -1380,16 +1380,16 @@
         <v>70</v>
       </c>
       <c r="B15" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C15" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D15" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E15" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -1400,13 +1400,13 @@
         <v>0</v>
       </c>
       <c r="C16" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D16" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E16" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -1417,13 +1417,13 @@
         <v>0</v>
       </c>
       <c r="C17" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D17" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E17" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -1434,13 +1434,13 @@
         <v>0</v>
       </c>
       <c r="C18" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D18" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E18" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -1451,13 +1451,13 @@
         <v>0</v>
       </c>
       <c r="C19" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D19" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E19" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -1468,13 +1468,13 @@
         <v>0</v>
       </c>
       <c r="C20" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D20" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E20" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -1485,13 +1485,13 @@
         <v>0</v>
       </c>
       <c r="C21" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D21" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E21" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -1502,13 +1502,13 @@
         <v>0</v>
       </c>
       <c r="C22" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D22" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E22" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -1519,13 +1519,13 @@
         <v>0</v>
       </c>
       <c r="C23" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D23" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E23" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -1536,13 +1536,13 @@
         <v>0</v>
       </c>
       <c r="C24" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D24" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E24" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added reset test result function
</commit_message>
<xml_diff>
--- a/Connected Office Web Application User Acceptance Test/Connected Office Test Data.xlsx
+++ b/Connected Office Web Application User Acceptance Test/Connected Office Test Data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marcel\Desktop\323 P4\CMPG-323-Project-4---35376759\Connected Office Web Application User Acceptance Test\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marcel\Desktop\New folder\CMPG-323-Project-4---35376759\Connected Office Web Application User Acceptance Test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B7A91DB-3554-421D-A5A6-A29A7E2D1E39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8A32C47-297E-43FD-9BE6-1E2CB6AAC241}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="660" yWindow="1455" windowWidth="23850" windowHeight="11295" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Device" sheetId="1" r:id="rId1"/>
@@ -1126,7 +1126,7 @@
   <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1159,16 +1159,16 @@
         <v>57</v>
       </c>
       <c r="B2" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D2" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E2" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1176,16 +1176,16 @@
         <v>58</v>
       </c>
       <c r="B3" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C3" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D3" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E3" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -1193,16 +1193,16 @@
         <v>59</v>
       </c>
       <c r="B4" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C4" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D4" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E4" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1210,16 +1210,16 @@
         <v>60</v>
       </c>
       <c r="B5" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C5" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D5" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E5" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -1227,16 +1227,16 @@
         <v>61</v>
       </c>
       <c r="B6" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C6" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D6" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E6" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -1244,16 +1244,16 @@
         <v>62</v>
       </c>
       <c r="B7" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C7" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D7" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E7" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -1261,16 +1261,16 @@
         <v>63</v>
       </c>
       <c r="B8" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C8" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D8" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E8" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -1278,16 +1278,16 @@
         <v>64</v>
       </c>
       <c r="B9" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C9" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D9" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E9" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -1295,16 +1295,16 @@
         <v>65</v>
       </c>
       <c r="B10" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C10" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D10" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E10" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -1312,16 +1312,16 @@
         <v>66</v>
       </c>
       <c r="B11" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C11" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D11" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E11" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -1329,16 +1329,16 @@
         <v>67</v>
       </c>
       <c r="B12" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C12" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D12" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E12" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -1346,16 +1346,16 @@
         <v>68</v>
       </c>
       <c r="B13" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C13" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D13" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E13" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -1363,16 +1363,16 @@
         <v>69</v>
       </c>
       <c r="B14" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C14" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D14" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E14" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -1380,16 +1380,16 @@
         <v>70</v>
       </c>
       <c r="B15" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C15" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D15" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E15" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -1400,13 +1400,13 @@
         <v>0</v>
       </c>
       <c r="C16" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D16" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E16" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -1417,13 +1417,13 @@
         <v>0</v>
       </c>
       <c r="C17" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D17" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E17" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -1434,13 +1434,13 @@
         <v>0</v>
       </c>
       <c r="C18" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D18" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E18" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -1451,13 +1451,13 @@
         <v>0</v>
       </c>
       <c r="C19" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D19" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E19" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -1468,13 +1468,13 @@
         <v>0</v>
       </c>
       <c r="C20" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D20" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E20" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -1485,13 +1485,13 @@
         <v>0</v>
       </c>
       <c r="C21" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D21" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E21" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -1502,13 +1502,13 @@
         <v>0</v>
       </c>
       <c r="C22" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D22" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E22" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -1519,13 +1519,13 @@
         <v>0</v>
       </c>
       <c r="C23" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D23" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E23" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -1536,13 +1536,13 @@
         <v>0</v>
       </c>
       <c r="C24" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D24" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E24" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Final commit project 4
</commit_message>
<xml_diff>
--- a/Connected Office Web Application User Acceptance Test/Connected Office Test Data.xlsx
+++ b/Connected Office Web Application User Acceptance Test/Connected Office Test Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marcel\Desktop\New folder\CMPG-323-Project-4---35376759\Connected Office Web Application User Acceptance Test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8A32C47-297E-43FD-9BE6-1E2CB6AAC241}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DD1F309-BED6-4B5C-9EDC-E6CDE07E73E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="660" yWindow="1455" windowWidth="23850" windowHeight="11295" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1125,8 +1125,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{243FE4D3-E987-44A9-BA20-E766DD09E091}">
   <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1159,16 +1159,16 @@
         <v>57</v>
       </c>
       <c r="B2" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D2" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E2" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1176,16 +1176,16 @@
         <v>58</v>
       </c>
       <c r="B3" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C3" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D3" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E3" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -1193,16 +1193,16 @@
         <v>59</v>
       </c>
       <c r="B4" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C4" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D4" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E4" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1210,16 +1210,16 @@
         <v>60</v>
       </c>
       <c r="B5" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C5" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D5" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E5" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -1227,16 +1227,16 @@
         <v>61</v>
       </c>
       <c r="B6" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C6" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D6" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E6" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -1244,16 +1244,16 @@
         <v>62</v>
       </c>
       <c r="B7" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C7" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D7" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E7" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -1261,16 +1261,16 @@
         <v>63</v>
       </c>
       <c r="B8" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C8" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D8" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E8" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -1278,16 +1278,16 @@
         <v>64</v>
       </c>
       <c r="B9" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C9" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D9" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E9" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -1295,16 +1295,16 @@
         <v>65</v>
       </c>
       <c r="B10" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C10" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D10" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E10" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -1312,16 +1312,16 @@
         <v>66</v>
       </c>
       <c r="B11" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C11" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D11" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E11" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -1329,16 +1329,16 @@
         <v>67</v>
       </c>
       <c r="B12" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C12" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D12" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E12" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -1346,16 +1346,16 @@
         <v>68</v>
       </c>
       <c r="B13" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C13" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D13" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E13" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -1363,16 +1363,16 @@
         <v>69</v>
       </c>
       <c r="B14" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C14" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D14" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E14" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -1380,16 +1380,16 @@
         <v>70</v>
       </c>
       <c r="B15" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C15" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D15" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E15" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -1400,13 +1400,13 @@
         <v>0</v>
       </c>
       <c r="C16" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D16" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E16" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -1417,13 +1417,13 @@
         <v>0</v>
       </c>
       <c r="C17" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D17" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E17" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -1434,13 +1434,13 @@
         <v>0</v>
       </c>
       <c r="C18" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D18" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E18" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -1451,13 +1451,13 @@
         <v>0</v>
       </c>
       <c r="C19" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D19" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E19" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -1468,13 +1468,13 @@
         <v>0</v>
       </c>
       <c r="C20" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D20" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E20" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -1485,13 +1485,13 @@
         <v>0</v>
       </c>
       <c r="C21" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D21" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E21" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -1502,13 +1502,13 @@
         <v>0</v>
       </c>
       <c r="C22" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D22" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E22" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -1519,13 +1519,13 @@
         <v>0</v>
       </c>
       <c r="C23" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D23" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E23" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -1536,10 +1536,10 @@
         <v>0</v>
       </c>
       <c r="C24" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D24" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E24" s="2" t="b">
         <v>0</v>

</xml_diff>

<commit_message>
Added a main workflow that invokes all the other methods
</commit_message>
<xml_diff>
--- a/Connected Office Web Application User Acceptance Test/Connected Office Test Data.xlsx
+++ b/Connected Office Web Application User Acceptance Test/Connected Office Test Data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marcel\Desktop\New folder\CMPG-323-Project-4---35376759\Connected Office Web Application User Acceptance Test\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marcel\Desktop\323\Project 4\CMPG-323-Project-4---35376759\Connected Office Web Application User Acceptance Test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DD1F309-BED6-4B5C-9EDC-E6CDE07E73E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D06AD011-C1AF-43E5-84FA-25449D9F0563}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="660" yWindow="1455" windowWidth="23850" windowHeight="11295" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="660" yWindow="1455" windowWidth="23850" windowHeight="11295" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Device" sheetId="1" r:id="rId1"/>
@@ -1123,10 +1123,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{243FE4D3-E987-44A9-BA20-E766DD09E091}">
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="M18" sqref="M18"/>
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1542,7 +1542,73 @@
         <v>1</v>
       </c>
       <c r="E24" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C25" t="b">
+        <v>1</v>
+      </c>
+      <c r="E25" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C26" t="b">
+        <v>1</v>
+      </c>
+      <c r="E26" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C27" t="b">
+        <v>1</v>
+      </c>
+      <c r="E27" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C28" t="b">
+        <v>1</v>
+      </c>
+      <c r="E28" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C29" t="b">
+        <v>1</v>
+      </c>
+      <c r="E29" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C30" t="b">
+        <v>1</v>
+      </c>
+      <c r="E30" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C31" t="b">
+        <v>1</v>
+      </c>
+      <c r="E31" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C32" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C33" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>